<commit_message>
Added example of how to use numpy
</commit_message>
<xml_diff>
--- a/xls/ExPyExamples.xlsx
+++ b/xls/ExPyExamples.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RegEx" sheetId="1" r:id="rId1"/>
+    <sheet name="use numpy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,10 +24,95 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+  <si>
+    <t>import ExPy;</t>
+  </si>
+  <si>
+    <t>import sys;</t>
+  </si>
+  <si>
+    <t>sys.path.append("F:\\")</t>
+  </si>
+  <si>
+    <t>ExPy.Splash()</t>
+  </si>
+  <si>
+    <t>ExPy.__version__</t>
+  </si>
+  <si>
+    <t>import re;</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>ExPy.register(mfnnn3,1)</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>1f</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def mfnnn3(s):
+   return str(re.compile("^[0-9a-e]+$").match(str(s)))
+</t>
+  </si>
+  <si>
+    <t>xf</t>
+  </si>
+  <si>
+    <t>29384</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>mfnnn3</t>
+  </si>
+  <si>
+    <t>Example of Regular Expressions in Excel</t>
+  </si>
+  <si>
+    <t>numpy.random.random()</t>
+  </si>
+  <si>
+    <t>ExPy.register(npeigv,1)</t>
+  </si>
+  <si>
+    <t>def npeigv(x) :
+   return numpy.linalg.eigvals(numpy.array(x.array()))</t>
+  </si>
+  <si>
+    <t>Note that paramter x must be converted by the use of the .array() method</t>
+  </si>
+  <si>
+    <t>import numpy; import scipy;</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,8 +140,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +429,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="57" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="29" max="29" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>_xll.ExPyScript(A2)</f>
+        <v>None</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="str">
+        <f>_xll.ExPyEvalSS(D2)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>_xll.ExPyScript(A3)</f>
+        <v>&lt;NULL&gt;</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.ExPyEvalSS(D3)</f>
+        <v>&lt;function mfnnn3 at 0x0D5333F0&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="str">
+        <f>_xll.ExPyScript(A4)</f>
+        <v>None</v>
+      </c>
+      <c r="E4" t="str">
+        <f>_xll.ExPyEvalSS(D4)</f>
+        <v>&lt;NULL&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="str">
+        <f>_xll.ExPyScript(A5)</f>
+        <v>None</v>
+      </c>
+      <c r="E5" t="str">
+        <f>_xll.ExPyEvalSS(D5)</f>
+        <v>&lt;NULL&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>_xll.ExPyScript(A6)</f>
+        <v>None</v>
+      </c>
+      <c r="E6" t="str">
+        <f>_xll.ExPyEvalSS(D6)</f>
+        <v>&lt;NULL&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="str">
+        <f>_xll.ExPyScript(A7)</f>
+        <v>None</v>
+      </c>
+      <c r="E7" t="str">
+        <f>_xll.ExPyEvalSS(D7)</f>
+        <v>&lt;NULL&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="str">
+        <f>_xll.ExPyScript(A8)</f>
+        <v>None</v>
+      </c>
+      <c r="E8" t="str">
+        <f>_xll.ExPyEvalSS(D8)</f>
+        <v>&lt;NULL&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" t="str">
+        <f>_xll.ExPyEvalSS(D9)</f>
+        <v>&lt;NULL&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xll.mfnnn3(B11)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xll.mfnnn3(B12)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xll.mfnnn3(B13)</f>
+        <v>None</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="str">
+        <f>_xll.mfnnn3(B14)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="str">
+        <f>_xll.mfnnn3(B15)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="str">
+        <f>_xll.mfnnn3(B16)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="str">
+        <f>_xll.mfnnn3(B17)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="str">
+        <f>_xll.mfnnn3(B18)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="str">
+        <f>_xll.mfnnn3(B19)</f>
+        <v>None</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="str">
+        <f>_xll.mfnnn3(B20)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="str">
+        <f>_xll.mfnnn3(B21)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="str">
+        <f>_xll.mfnnn3(B22)</f>
+        <v>&lt;_sre.SRE_Match object at 0x0D4D9B48&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>_xll.ExPyScript(B1)</f>
+        <v>None</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xll.ExPyScript(B2)</f>
+        <v>None</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xll.ExPyEvalSS(E2)</f>
+        <v>0.152423536066</v>
+      </c>
+      <c r="J2">
+        <f>SIN(F2)</f>
+        <v>0.15183401363194202</v>
+      </c>
+      <c r="K2">
+        <f>COS(F2)</f>
+        <v>0.98840600580146987</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xll.ExPyScript(B3)</f>
+        <v>None</v>
+      </c>
+      <c r="J3">
+        <f>COS(F2)</f>
+        <v>0.98840600580146987</v>
+      </c>
+      <c r="K3">
+        <f>SIN(F2)</f>
+        <v>0.15183401363194202</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <f>_xll.ExPyScript(B4)</f>
+        <v>None</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xll.ExPyScript(B5)</f>
+        <v>None</v>
+      </c>
+      <c r="F5">
+        <f t="array" ref="F5:F6">_xll.npeigv(J2:K3)</f>
+        <v>1.1402400194334119</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="str">
+        <f>_xll.ExPyScript(B6)</f>
+        <v>None</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>-0.83657199216952782</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xll.ExPyScript(B7)</f>
+        <v>None</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Automatically add the path of the addin file to the Python path so that .py files are found easily
</commit_message>
<xml_diff>
--- a/xls/ExPyExamples.xlsx
+++ b/xls/ExPyExamples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="RegEx" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
-  <si>
-    <t>import ExPy;</t>
-  </si>
-  <si>
-    <t>import sys;</t>
-  </si>
-  <si>
-    <t>sys.path.append("F:\\")</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>ExPy.Splash()</t>
   </si>
@@ -431,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +436,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -455,15 +446,8 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <f>_xll.ExPyScript(A2)</f>
-        <v>None</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
       </c>
       <c r="E2" t="str">
         <f>_xll.ExPyEvalSS(D2)</f>
@@ -471,15 +455,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <f>_xll.ExPyScript(A3)</f>
-        <v>&lt;NULL&gt;</v>
-      </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" t="str">
         <f>_xll.ExPyEvalSS(D3)</f>
@@ -487,13 +464,6 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="str">
-        <f>_xll.ExPyScript(A4)</f>
-        <v>None</v>
-      </c>
       <c r="E4" t="str">
         <f>_xll.ExPyEvalSS(D4)</f>
         <v>&lt;NULL&gt;</v>
@@ -501,7 +471,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="str">
         <f>_xll.ExPyScript(A5)</f>
@@ -514,7 +484,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="str">
         <f>_xll.ExPyScript(A6)</f>
@@ -527,7 +497,7 @@
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="str">
         <f>_xll.ExPyScript(A7)</f>
@@ -540,7 +510,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" t="str">
         <f>_xll.ExPyScript(A8)</f>
@@ -559,7 +529,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" t="str">
         <f>_xll.mfnnn3(B11)</f>
@@ -568,7 +538,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C12" t="str">
         <f>_xll.mfnnn3(B12)</f>
@@ -577,7 +547,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C13" t="str">
         <f>_xll.mfnnn3(B13)</f>
@@ -586,7 +556,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" t="str">
         <f>_xll.mfnnn3(B14)</f>
@@ -595,7 +565,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C15" t="str">
         <f>_xll.mfnnn3(B15)</f>
@@ -604,7 +574,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C16" t="str">
         <f>_xll.mfnnn3(B16)</f>
@@ -613,7 +583,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C17" t="str">
         <f>_xll.mfnnn3(B17)</f>
@@ -622,7 +592,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18" t="str">
         <f>_xll.mfnnn3(B18)</f>
@@ -631,7 +601,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19" t="str">
         <f>_xll.mfnnn3(B19)</f>
@@ -640,7 +610,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C20" t="str">
         <f>_xll.mfnnn3(B20)</f>
@@ -649,7 +619,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C21" t="str">
         <f>_xll.mfnnn3(B21)</f>
@@ -658,7 +628,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C22" t="str">
         <f>_xll.mfnnn3(B22)</f>
@@ -676,11 +646,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K7"/>
+  <dimension ref="B2:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -690,59 +658,36 @@
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="str">
-        <f>_xll.ExPyScript(B1)</f>
-        <v>None</v>
-      </c>
-    </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="str">
-        <f>_xll.ExPyScript(B2)</f>
-        <v>None</v>
-      </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" t="str">
         <f>_xll.ExPyEvalSS(E2)</f>
-        <v>0.152423536066</v>
+        <v>0.575856781696</v>
       </c>
       <c r="J2">
         <f>SIN(F2)</f>
-        <v>0.15183401363194202</v>
+        <v>0.54455359559209782</v>
       </c>
       <c r="K2">
         <f>COS(F2)</f>
-        <v>0.98840600580146987</v>
+        <v>0.83872604676838192</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="str">
-        <f>_xll.ExPyScript(B3)</f>
-        <v>None</v>
-      </c>
       <c r="J3">
         <f>COS(F2)</f>
-        <v>0.98840600580146987</v>
+        <v>0.83872604676838192</v>
       </c>
       <c r="K3">
         <f>SIN(F2)</f>
-        <v>0.15183401363194202</v>
+        <v>0.54455359559209782</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" t="str">
         <f>_xll.ExPyScript(B4)</f>
@@ -751,7 +696,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" t="str">
         <f>_xll.ExPyScript(B5)</f>
@@ -759,27 +704,27 @@
       </c>
       <c r="F5">
         <f t="array" ref="F5:F6">_xll.npeigv(J2:K3)</f>
-        <v>1.1402400194334119</v>
+        <v>1.3832796423604798</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="str">
         <f>_xll.ExPyScript(B6)</f>
         <v>None</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6">
-        <v>-0.83657199216952782</v>
+        <v>-0.2941724511762841</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="str">
         <f>_xll.ExPyScript(B7)</f>

</xml_diff>